<commit_message>
Added deployment 2 data for Irminger FLMA/B and HYPM
Added deployment 2 data for Irminger FLMA/B and HYPM
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI02HYPM_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GI02HYPM_00002.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
   <si>
     <t>Ref Des</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>GI02HYPM-WFP02-00-WFPENG000</t>
+  </si>
+  <si>
+    <t>OL000024</t>
   </si>
 </sst>
 </file>
@@ -1529,7 +1532,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2178,7 +2181,9 @@
       <c r="D28" s="3">
         <v>2</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="F28" s="51">
         <v>13284</v>
       </c>

</xml_diff>